<commit_message>
Adding Exp-1-b.xlsx in Assignment_48_Exp1-b
</commit_message>
<xml_diff>
--- a/Assignment_48_Exp1-b/Exp-1-b.xlsx
+++ b/Assignment_48_Exp1-b/Exp-1-b.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\DAA\Assignment_48_Exp1-b\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7304D22C-529F-4FE8-985A-DA030C893E2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035E2735-427E-4723-83E5-7ED9FFF73CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6485B1F8-7EE5-468E-A22C-62769FE0806F}"/>
   </bookViews>
@@ -123,21 +123,41 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="3.9303504427338203E-2"/>
-          <c:y val="0.1301234475139631"/>
-          <c:w val="0.92396598606079228"/>
-          <c:h val="0.75232306616406652"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -167,10 +187,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$839</c:f>
+              <c:f>Sheet1!$A$2:$A$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="838"/>
+                <c:ptCount val="1000"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -2684,16 +2704,502 @@
                 </c:pt>
                 <c:pt idx="837">
                   <c:v>83800</c:v>
+                </c:pt>
+                <c:pt idx="838">
+                  <c:v>83900</c:v>
+                </c:pt>
+                <c:pt idx="839">
+                  <c:v>84000</c:v>
+                </c:pt>
+                <c:pt idx="840">
+                  <c:v>84100</c:v>
+                </c:pt>
+                <c:pt idx="841">
+                  <c:v>84200</c:v>
+                </c:pt>
+                <c:pt idx="842">
+                  <c:v>84300</c:v>
+                </c:pt>
+                <c:pt idx="843">
+                  <c:v>84400</c:v>
+                </c:pt>
+                <c:pt idx="844">
+                  <c:v>84500</c:v>
+                </c:pt>
+                <c:pt idx="845">
+                  <c:v>84600</c:v>
+                </c:pt>
+                <c:pt idx="846">
+                  <c:v>84700</c:v>
+                </c:pt>
+                <c:pt idx="847">
+                  <c:v>84800</c:v>
+                </c:pt>
+                <c:pt idx="848">
+                  <c:v>84900</c:v>
+                </c:pt>
+                <c:pt idx="849">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="850">
+                  <c:v>85100</c:v>
+                </c:pt>
+                <c:pt idx="851">
+                  <c:v>85200</c:v>
+                </c:pt>
+                <c:pt idx="852">
+                  <c:v>85300</c:v>
+                </c:pt>
+                <c:pt idx="853">
+                  <c:v>85400</c:v>
+                </c:pt>
+                <c:pt idx="854">
+                  <c:v>85500</c:v>
+                </c:pt>
+                <c:pt idx="855">
+                  <c:v>85600</c:v>
+                </c:pt>
+                <c:pt idx="856">
+                  <c:v>85700</c:v>
+                </c:pt>
+                <c:pt idx="857">
+                  <c:v>85800</c:v>
+                </c:pt>
+                <c:pt idx="858">
+                  <c:v>85900</c:v>
+                </c:pt>
+                <c:pt idx="859">
+                  <c:v>86000</c:v>
+                </c:pt>
+                <c:pt idx="860">
+                  <c:v>86100</c:v>
+                </c:pt>
+                <c:pt idx="861">
+                  <c:v>86200</c:v>
+                </c:pt>
+                <c:pt idx="862">
+                  <c:v>86300</c:v>
+                </c:pt>
+                <c:pt idx="863">
+                  <c:v>86400</c:v>
+                </c:pt>
+                <c:pt idx="864">
+                  <c:v>86500</c:v>
+                </c:pt>
+                <c:pt idx="865">
+                  <c:v>86600</c:v>
+                </c:pt>
+                <c:pt idx="866">
+                  <c:v>86700</c:v>
+                </c:pt>
+                <c:pt idx="867">
+                  <c:v>86800</c:v>
+                </c:pt>
+                <c:pt idx="868">
+                  <c:v>86900</c:v>
+                </c:pt>
+                <c:pt idx="869">
+                  <c:v>87000</c:v>
+                </c:pt>
+                <c:pt idx="870">
+                  <c:v>87100</c:v>
+                </c:pt>
+                <c:pt idx="871">
+                  <c:v>87200</c:v>
+                </c:pt>
+                <c:pt idx="872">
+                  <c:v>87300</c:v>
+                </c:pt>
+                <c:pt idx="873">
+                  <c:v>87400</c:v>
+                </c:pt>
+                <c:pt idx="874">
+                  <c:v>87500</c:v>
+                </c:pt>
+                <c:pt idx="875">
+                  <c:v>87600</c:v>
+                </c:pt>
+                <c:pt idx="876">
+                  <c:v>87700</c:v>
+                </c:pt>
+                <c:pt idx="877">
+                  <c:v>87800</c:v>
+                </c:pt>
+                <c:pt idx="878">
+                  <c:v>87900</c:v>
+                </c:pt>
+                <c:pt idx="879">
+                  <c:v>88000</c:v>
+                </c:pt>
+                <c:pt idx="880">
+                  <c:v>88100</c:v>
+                </c:pt>
+                <c:pt idx="881">
+                  <c:v>88200</c:v>
+                </c:pt>
+                <c:pt idx="882">
+                  <c:v>88300</c:v>
+                </c:pt>
+                <c:pt idx="883">
+                  <c:v>88400</c:v>
+                </c:pt>
+                <c:pt idx="884">
+                  <c:v>88500</c:v>
+                </c:pt>
+                <c:pt idx="885">
+                  <c:v>88600</c:v>
+                </c:pt>
+                <c:pt idx="886">
+                  <c:v>88700</c:v>
+                </c:pt>
+                <c:pt idx="887">
+                  <c:v>88800</c:v>
+                </c:pt>
+                <c:pt idx="888">
+                  <c:v>88900</c:v>
+                </c:pt>
+                <c:pt idx="889">
+                  <c:v>89000</c:v>
+                </c:pt>
+                <c:pt idx="890">
+                  <c:v>89100</c:v>
+                </c:pt>
+                <c:pt idx="891">
+                  <c:v>89200</c:v>
+                </c:pt>
+                <c:pt idx="892">
+                  <c:v>89300</c:v>
+                </c:pt>
+                <c:pt idx="893">
+                  <c:v>89400</c:v>
+                </c:pt>
+                <c:pt idx="894">
+                  <c:v>89500</c:v>
+                </c:pt>
+                <c:pt idx="895">
+                  <c:v>89600</c:v>
+                </c:pt>
+                <c:pt idx="896">
+                  <c:v>89700</c:v>
+                </c:pt>
+                <c:pt idx="897">
+                  <c:v>89800</c:v>
+                </c:pt>
+                <c:pt idx="898">
+                  <c:v>89900</c:v>
+                </c:pt>
+                <c:pt idx="899">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="900">
+                  <c:v>90100</c:v>
+                </c:pt>
+                <c:pt idx="901">
+                  <c:v>90200</c:v>
+                </c:pt>
+                <c:pt idx="902">
+                  <c:v>90300</c:v>
+                </c:pt>
+                <c:pt idx="903">
+                  <c:v>90400</c:v>
+                </c:pt>
+                <c:pt idx="904">
+                  <c:v>90500</c:v>
+                </c:pt>
+                <c:pt idx="905">
+                  <c:v>90600</c:v>
+                </c:pt>
+                <c:pt idx="906">
+                  <c:v>90700</c:v>
+                </c:pt>
+                <c:pt idx="907">
+                  <c:v>90800</c:v>
+                </c:pt>
+                <c:pt idx="908">
+                  <c:v>90900</c:v>
+                </c:pt>
+                <c:pt idx="909">
+                  <c:v>91000</c:v>
+                </c:pt>
+                <c:pt idx="910">
+                  <c:v>91100</c:v>
+                </c:pt>
+                <c:pt idx="911">
+                  <c:v>91200</c:v>
+                </c:pt>
+                <c:pt idx="912">
+                  <c:v>91300</c:v>
+                </c:pt>
+                <c:pt idx="913">
+                  <c:v>91400</c:v>
+                </c:pt>
+                <c:pt idx="914">
+                  <c:v>91500</c:v>
+                </c:pt>
+                <c:pt idx="915">
+                  <c:v>91600</c:v>
+                </c:pt>
+                <c:pt idx="916">
+                  <c:v>91700</c:v>
+                </c:pt>
+                <c:pt idx="917">
+                  <c:v>91800</c:v>
+                </c:pt>
+                <c:pt idx="918">
+                  <c:v>91900</c:v>
+                </c:pt>
+                <c:pt idx="919">
+                  <c:v>92000</c:v>
+                </c:pt>
+                <c:pt idx="920">
+                  <c:v>92100</c:v>
+                </c:pt>
+                <c:pt idx="921">
+                  <c:v>92200</c:v>
+                </c:pt>
+                <c:pt idx="922">
+                  <c:v>92300</c:v>
+                </c:pt>
+                <c:pt idx="923">
+                  <c:v>92400</c:v>
+                </c:pt>
+                <c:pt idx="924">
+                  <c:v>92500</c:v>
+                </c:pt>
+                <c:pt idx="925">
+                  <c:v>92600</c:v>
+                </c:pt>
+                <c:pt idx="926">
+                  <c:v>92700</c:v>
+                </c:pt>
+                <c:pt idx="927">
+                  <c:v>92800</c:v>
+                </c:pt>
+                <c:pt idx="928">
+                  <c:v>92900</c:v>
+                </c:pt>
+                <c:pt idx="929">
+                  <c:v>93000</c:v>
+                </c:pt>
+                <c:pt idx="930">
+                  <c:v>93100</c:v>
+                </c:pt>
+                <c:pt idx="931">
+                  <c:v>93200</c:v>
+                </c:pt>
+                <c:pt idx="932">
+                  <c:v>93300</c:v>
+                </c:pt>
+                <c:pt idx="933">
+                  <c:v>93400</c:v>
+                </c:pt>
+                <c:pt idx="934">
+                  <c:v>93500</c:v>
+                </c:pt>
+                <c:pt idx="935">
+                  <c:v>93600</c:v>
+                </c:pt>
+                <c:pt idx="936">
+                  <c:v>93700</c:v>
+                </c:pt>
+                <c:pt idx="937">
+                  <c:v>93800</c:v>
+                </c:pt>
+                <c:pt idx="938">
+                  <c:v>93900</c:v>
+                </c:pt>
+                <c:pt idx="939">
+                  <c:v>94000</c:v>
+                </c:pt>
+                <c:pt idx="940">
+                  <c:v>94100</c:v>
+                </c:pt>
+                <c:pt idx="941">
+                  <c:v>94200</c:v>
+                </c:pt>
+                <c:pt idx="942">
+                  <c:v>94300</c:v>
+                </c:pt>
+                <c:pt idx="943">
+                  <c:v>94400</c:v>
+                </c:pt>
+                <c:pt idx="944">
+                  <c:v>94500</c:v>
+                </c:pt>
+                <c:pt idx="945">
+                  <c:v>94600</c:v>
+                </c:pt>
+                <c:pt idx="946">
+                  <c:v>94700</c:v>
+                </c:pt>
+                <c:pt idx="947">
+                  <c:v>94800</c:v>
+                </c:pt>
+                <c:pt idx="948">
+                  <c:v>94900</c:v>
+                </c:pt>
+                <c:pt idx="949">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="950">
+                  <c:v>95100</c:v>
+                </c:pt>
+                <c:pt idx="951">
+                  <c:v>95200</c:v>
+                </c:pt>
+                <c:pt idx="952">
+                  <c:v>95300</c:v>
+                </c:pt>
+                <c:pt idx="953">
+                  <c:v>95400</c:v>
+                </c:pt>
+                <c:pt idx="954">
+                  <c:v>95500</c:v>
+                </c:pt>
+                <c:pt idx="955">
+                  <c:v>95600</c:v>
+                </c:pt>
+                <c:pt idx="956">
+                  <c:v>95700</c:v>
+                </c:pt>
+                <c:pt idx="957">
+                  <c:v>95800</c:v>
+                </c:pt>
+                <c:pt idx="958">
+                  <c:v>95900</c:v>
+                </c:pt>
+                <c:pt idx="959">
+                  <c:v>96000</c:v>
+                </c:pt>
+                <c:pt idx="960">
+                  <c:v>96100</c:v>
+                </c:pt>
+                <c:pt idx="961">
+                  <c:v>96200</c:v>
+                </c:pt>
+                <c:pt idx="962">
+                  <c:v>96300</c:v>
+                </c:pt>
+                <c:pt idx="963">
+                  <c:v>96400</c:v>
+                </c:pt>
+                <c:pt idx="964">
+                  <c:v>96500</c:v>
+                </c:pt>
+                <c:pt idx="965">
+                  <c:v>96600</c:v>
+                </c:pt>
+                <c:pt idx="966">
+                  <c:v>96700</c:v>
+                </c:pt>
+                <c:pt idx="967">
+                  <c:v>96800</c:v>
+                </c:pt>
+                <c:pt idx="968">
+                  <c:v>96900</c:v>
+                </c:pt>
+                <c:pt idx="969">
+                  <c:v>97000</c:v>
+                </c:pt>
+                <c:pt idx="970">
+                  <c:v>97100</c:v>
+                </c:pt>
+                <c:pt idx="971">
+                  <c:v>97200</c:v>
+                </c:pt>
+                <c:pt idx="972">
+                  <c:v>97300</c:v>
+                </c:pt>
+                <c:pt idx="973">
+                  <c:v>97400</c:v>
+                </c:pt>
+                <c:pt idx="974">
+                  <c:v>97500</c:v>
+                </c:pt>
+                <c:pt idx="975">
+                  <c:v>97600</c:v>
+                </c:pt>
+                <c:pt idx="976">
+                  <c:v>97700</c:v>
+                </c:pt>
+                <c:pt idx="977">
+                  <c:v>97800</c:v>
+                </c:pt>
+                <c:pt idx="978">
+                  <c:v>97900</c:v>
+                </c:pt>
+                <c:pt idx="979">
+                  <c:v>98000</c:v>
+                </c:pt>
+                <c:pt idx="980">
+                  <c:v>98100</c:v>
+                </c:pt>
+                <c:pt idx="981">
+                  <c:v>98200</c:v>
+                </c:pt>
+                <c:pt idx="982">
+                  <c:v>98300</c:v>
+                </c:pt>
+                <c:pt idx="983">
+                  <c:v>98400</c:v>
+                </c:pt>
+                <c:pt idx="984">
+                  <c:v>98500</c:v>
+                </c:pt>
+                <c:pt idx="985">
+                  <c:v>98600</c:v>
+                </c:pt>
+                <c:pt idx="986">
+                  <c:v>98700</c:v>
+                </c:pt>
+                <c:pt idx="987">
+                  <c:v>98800</c:v>
+                </c:pt>
+                <c:pt idx="988">
+                  <c:v>98900</c:v>
+                </c:pt>
+                <c:pt idx="989">
+                  <c:v>99000</c:v>
+                </c:pt>
+                <c:pt idx="990">
+                  <c:v>99100</c:v>
+                </c:pt>
+                <c:pt idx="991">
+                  <c:v>99200</c:v>
+                </c:pt>
+                <c:pt idx="992">
+                  <c:v>99300</c:v>
+                </c:pt>
+                <c:pt idx="993">
+                  <c:v>99400</c:v>
+                </c:pt>
+                <c:pt idx="994">
+                  <c:v>99500</c:v>
+                </c:pt>
+                <c:pt idx="995">
+                  <c:v>99600</c:v>
+                </c:pt>
+                <c:pt idx="996">
+                  <c:v>99700</c:v>
+                </c:pt>
+                <c:pt idx="997">
+                  <c:v>99800</c:v>
+                </c:pt>
+                <c:pt idx="998">
+                  <c:v>99900</c:v>
+                </c:pt>
+                <c:pt idx="999">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$839</c:f>
+              <c:f>Sheet1!$B$2:$B$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="838"/>
+                <c:ptCount val="1000"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5207,14 +5713,500 @@
                 </c:pt>
                 <c:pt idx="837">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="838">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="839">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="840">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="841">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="842">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="843">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="844">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="845">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="846">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="847">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="848">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="849">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="850">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="851">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="852">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="853">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="854">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="855">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="856">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="857">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="858">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="859">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="860">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="861">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="862">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="863">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="864">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="865">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="866">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="867">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="868">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="869">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="870">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="871">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="872">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="873">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="874">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="875">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="876">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="877">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="878">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="879">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="880">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="881">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="882">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="883">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="884">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="885">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="886">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="887">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="888">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="889">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="890">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="891">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="892">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="893">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="894">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="895">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="896">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="897">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="898">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="899">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="900">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="901">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="902">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="903">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="904">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="905">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="906">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="907">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="908">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="909">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="910">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="911">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="912">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="913">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="914">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="915">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="916">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="917">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="918">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="919">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="920">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="921">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="922">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="923">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="924">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="925">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="926">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="927">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="928">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="929">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="930">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="931">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="932">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="933">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="934">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="935">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="936">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="937">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="938">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="939">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="940">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="941">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="942">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="943">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="944">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="945">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="946">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="947">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="948">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="949">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="950">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="951">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="952">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="953">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="954">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="955">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="956">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="957">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="958">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="959">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="960">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="961">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="962">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="963">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="964">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="965">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="966">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="967">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="968">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="969">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="970">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="971">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="972">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="973">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="974">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="975">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="976">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="977">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="978">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="979">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="980">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="981">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="982">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="983">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="984">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="985">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="986">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="987">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="988">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="989">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="990">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="991">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="992">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="993">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="994">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="995">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="996">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="997">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="998">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="999">
+                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-16BF-4A92-9F12-241668F6DF81}"/>
+              <c16:uniqueId val="{00000000-4C15-459C-B3ED-C7353D9B3358}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5243,10 +6235,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$839</c:f>
+              <c:f>Sheet1!$A$2:$A$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="838"/>
+                <c:ptCount val="1000"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -7760,23 +8752,509 @@
                 </c:pt>
                 <c:pt idx="837">
                   <c:v>83800</c:v>
+                </c:pt>
+                <c:pt idx="838">
+                  <c:v>83900</c:v>
+                </c:pt>
+                <c:pt idx="839">
+                  <c:v>84000</c:v>
+                </c:pt>
+                <c:pt idx="840">
+                  <c:v>84100</c:v>
+                </c:pt>
+                <c:pt idx="841">
+                  <c:v>84200</c:v>
+                </c:pt>
+                <c:pt idx="842">
+                  <c:v>84300</c:v>
+                </c:pt>
+                <c:pt idx="843">
+                  <c:v>84400</c:v>
+                </c:pt>
+                <c:pt idx="844">
+                  <c:v>84500</c:v>
+                </c:pt>
+                <c:pt idx="845">
+                  <c:v>84600</c:v>
+                </c:pt>
+                <c:pt idx="846">
+                  <c:v>84700</c:v>
+                </c:pt>
+                <c:pt idx="847">
+                  <c:v>84800</c:v>
+                </c:pt>
+                <c:pt idx="848">
+                  <c:v>84900</c:v>
+                </c:pt>
+                <c:pt idx="849">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="850">
+                  <c:v>85100</c:v>
+                </c:pt>
+                <c:pt idx="851">
+                  <c:v>85200</c:v>
+                </c:pt>
+                <c:pt idx="852">
+                  <c:v>85300</c:v>
+                </c:pt>
+                <c:pt idx="853">
+                  <c:v>85400</c:v>
+                </c:pt>
+                <c:pt idx="854">
+                  <c:v>85500</c:v>
+                </c:pt>
+                <c:pt idx="855">
+                  <c:v>85600</c:v>
+                </c:pt>
+                <c:pt idx="856">
+                  <c:v>85700</c:v>
+                </c:pt>
+                <c:pt idx="857">
+                  <c:v>85800</c:v>
+                </c:pt>
+                <c:pt idx="858">
+                  <c:v>85900</c:v>
+                </c:pt>
+                <c:pt idx="859">
+                  <c:v>86000</c:v>
+                </c:pt>
+                <c:pt idx="860">
+                  <c:v>86100</c:v>
+                </c:pt>
+                <c:pt idx="861">
+                  <c:v>86200</c:v>
+                </c:pt>
+                <c:pt idx="862">
+                  <c:v>86300</c:v>
+                </c:pt>
+                <c:pt idx="863">
+                  <c:v>86400</c:v>
+                </c:pt>
+                <c:pt idx="864">
+                  <c:v>86500</c:v>
+                </c:pt>
+                <c:pt idx="865">
+                  <c:v>86600</c:v>
+                </c:pt>
+                <c:pt idx="866">
+                  <c:v>86700</c:v>
+                </c:pt>
+                <c:pt idx="867">
+                  <c:v>86800</c:v>
+                </c:pt>
+                <c:pt idx="868">
+                  <c:v>86900</c:v>
+                </c:pt>
+                <c:pt idx="869">
+                  <c:v>87000</c:v>
+                </c:pt>
+                <c:pt idx="870">
+                  <c:v>87100</c:v>
+                </c:pt>
+                <c:pt idx="871">
+                  <c:v>87200</c:v>
+                </c:pt>
+                <c:pt idx="872">
+                  <c:v>87300</c:v>
+                </c:pt>
+                <c:pt idx="873">
+                  <c:v>87400</c:v>
+                </c:pt>
+                <c:pt idx="874">
+                  <c:v>87500</c:v>
+                </c:pt>
+                <c:pt idx="875">
+                  <c:v>87600</c:v>
+                </c:pt>
+                <c:pt idx="876">
+                  <c:v>87700</c:v>
+                </c:pt>
+                <c:pt idx="877">
+                  <c:v>87800</c:v>
+                </c:pt>
+                <c:pt idx="878">
+                  <c:v>87900</c:v>
+                </c:pt>
+                <c:pt idx="879">
+                  <c:v>88000</c:v>
+                </c:pt>
+                <c:pt idx="880">
+                  <c:v>88100</c:v>
+                </c:pt>
+                <c:pt idx="881">
+                  <c:v>88200</c:v>
+                </c:pt>
+                <c:pt idx="882">
+                  <c:v>88300</c:v>
+                </c:pt>
+                <c:pt idx="883">
+                  <c:v>88400</c:v>
+                </c:pt>
+                <c:pt idx="884">
+                  <c:v>88500</c:v>
+                </c:pt>
+                <c:pt idx="885">
+                  <c:v>88600</c:v>
+                </c:pt>
+                <c:pt idx="886">
+                  <c:v>88700</c:v>
+                </c:pt>
+                <c:pt idx="887">
+                  <c:v>88800</c:v>
+                </c:pt>
+                <c:pt idx="888">
+                  <c:v>88900</c:v>
+                </c:pt>
+                <c:pt idx="889">
+                  <c:v>89000</c:v>
+                </c:pt>
+                <c:pt idx="890">
+                  <c:v>89100</c:v>
+                </c:pt>
+                <c:pt idx="891">
+                  <c:v>89200</c:v>
+                </c:pt>
+                <c:pt idx="892">
+                  <c:v>89300</c:v>
+                </c:pt>
+                <c:pt idx="893">
+                  <c:v>89400</c:v>
+                </c:pt>
+                <c:pt idx="894">
+                  <c:v>89500</c:v>
+                </c:pt>
+                <c:pt idx="895">
+                  <c:v>89600</c:v>
+                </c:pt>
+                <c:pt idx="896">
+                  <c:v>89700</c:v>
+                </c:pt>
+                <c:pt idx="897">
+                  <c:v>89800</c:v>
+                </c:pt>
+                <c:pt idx="898">
+                  <c:v>89900</c:v>
+                </c:pt>
+                <c:pt idx="899">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="900">
+                  <c:v>90100</c:v>
+                </c:pt>
+                <c:pt idx="901">
+                  <c:v>90200</c:v>
+                </c:pt>
+                <c:pt idx="902">
+                  <c:v>90300</c:v>
+                </c:pt>
+                <c:pt idx="903">
+                  <c:v>90400</c:v>
+                </c:pt>
+                <c:pt idx="904">
+                  <c:v>90500</c:v>
+                </c:pt>
+                <c:pt idx="905">
+                  <c:v>90600</c:v>
+                </c:pt>
+                <c:pt idx="906">
+                  <c:v>90700</c:v>
+                </c:pt>
+                <c:pt idx="907">
+                  <c:v>90800</c:v>
+                </c:pt>
+                <c:pt idx="908">
+                  <c:v>90900</c:v>
+                </c:pt>
+                <c:pt idx="909">
+                  <c:v>91000</c:v>
+                </c:pt>
+                <c:pt idx="910">
+                  <c:v>91100</c:v>
+                </c:pt>
+                <c:pt idx="911">
+                  <c:v>91200</c:v>
+                </c:pt>
+                <c:pt idx="912">
+                  <c:v>91300</c:v>
+                </c:pt>
+                <c:pt idx="913">
+                  <c:v>91400</c:v>
+                </c:pt>
+                <c:pt idx="914">
+                  <c:v>91500</c:v>
+                </c:pt>
+                <c:pt idx="915">
+                  <c:v>91600</c:v>
+                </c:pt>
+                <c:pt idx="916">
+                  <c:v>91700</c:v>
+                </c:pt>
+                <c:pt idx="917">
+                  <c:v>91800</c:v>
+                </c:pt>
+                <c:pt idx="918">
+                  <c:v>91900</c:v>
+                </c:pt>
+                <c:pt idx="919">
+                  <c:v>92000</c:v>
+                </c:pt>
+                <c:pt idx="920">
+                  <c:v>92100</c:v>
+                </c:pt>
+                <c:pt idx="921">
+                  <c:v>92200</c:v>
+                </c:pt>
+                <c:pt idx="922">
+                  <c:v>92300</c:v>
+                </c:pt>
+                <c:pt idx="923">
+                  <c:v>92400</c:v>
+                </c:pt>
+                <c:pt idx="924">
+                  <c:v>92500</c:v>
+                </c:pt>
+                <c:pt idx="925">
+                  <c:v>92600</c:v>
+                </c:pt>
+                <c:pt idx="926">
+                  <c:v>92700</c:v>
+                </c:pt>
+                <c:pt idx="927">
+                  <c:v>92800</c:v>
+                </c:pt>
+                <c:pt idx="928">
+                  <c:v>92900</c:v>
+                </c:pt>
+                <c:pt idx="929">
+                  <c:v>93000</c:v>
+                </c:pt>
+                <c:pt idx="930">
+                  <c:v>93100</c:v>
+                </c:pt>
+                <c:pt idx="931">
+                  <c:v>93200</c:v>
+                </c:pt>
+                <c:pt idx="932">
+                  <c:v>93300</c:v>
+                </c:pt>
+                <c:pt idx="933">
+                  <c:v>93400</c:v>
+                </c:pt>
+                <c:pt idx="934">
+                  <c:v>93500</c:v>
+                </c:pt>
+                <c:pt idx="935">
+                  <c:v>93600</c:v>
+                </c:pt>
+                <c:pt idx="936">
+                  <c:v>93700</c:v>
+                </c:pt>
+                <c:pt idx="937">
+                  <c:v>93800</c:v>
+                </c:pt>
+                <c:pt idx="938">
+                  <c:v>93900</c:v>
+                </c:pt>
+                <c:pt idx="939">
+                  <c:v>94000</c:v>
+                </c:pt>
+                <c:pt idx="940">
+                  <c:v>94100</c:v>
+                </c:pt>
+                <c:pt idx="941">
+                  <c:v>94200</c:v>
+                </c:pt>
+                <c:pt idx="942">
+                  <c:v>94300</c:v>
+                </c:pt>
+                <c:pt idx="943">
+                  <c:v>94400</c:v>
+                </c:pt>
+                <c:pt idx="944">
+                  <c:v>94500</c:v>
+                </c:pt>
+                <c:pt idx="945">
+                  <c:v>94600</c:v>
+                </c:pt>
+                <c:pt idx="946">
+                  <c:v>94700</c:v>
+                </c:pt>
+                <c:pt idx="947">
+                  <c:v>94800</c:v>
+                </c:pt>
+                <c:pt idx="948">
+                  <c:v>94900</c:v>
+                </c:pt>
+                <c:pt idx="949">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="950">
+                  <c:v>95100</c:v>
+                </c:pt>
+                <c:pt idx="951">
+                  <c:v>95200</c:v>
+                </c:pt>
+                <c:pt idx="952">
+                  <c:v>95300</c:v>
+                </c:pt>
+                <c:pt idx="953">
+                  <c:v>95400</c:v>
+                </c:pt>
+                <c:pt idx="954">
+                  <c:v>95500</c:v>
+                </c:pt>
+                <c:pt idx="955">
+                  <c:v>95600</c:v>
+                </c:pt>
+                <c:pt idx="956">
+                  <c:v>95700</c:v>
+                </c:pt>
+                <c:pt idx="957">
+                  <c:v>95800</c:v>
+                </c:pt>
+                <c:pt idx="958">
+                  <c:v>95900</c:v>
+                </c:pt>
+                <c:pt idx="959">
+                  <c:v>96000</c:v>
+                </c:pt>
+                <c:pt idx="960">
+                  <c:v>96100</c:v>
+                </c:pt>
+                <c:pt idx="961">
+                  <c:v>96200</c:v>
+                </c:pt>
+                <c:pt idx="962">
+                  <c:v>96300</c:v>
+                </c:pt>
+                <c:pt idx="963">
+                  <c:v>96400</c:v>
+                </c:pt>
+                <c:pt idx="964">
+                  <c:v>96500</c:v>
+                </c:pt>
+                <c:pt idx="965">
+                  <c:v>96600</c:v>
+                </c:pt>
+                <c:pt idx="966">
+                  <c:v>96700</c:v>
+                </c:pt>
+                <c:pt idx="967">
+                  <c:v>96800</c:v>
+                </c:pt>
+                <c:pt idx="968">
+                  <c:v>96900</c:v>
+                </c:pt>
+                <c:pt idx="969">
+                  <c:v>97000</c:v>
+                </c:pt>
+                <c:pt idx="970">
+                  <c:v>97100</c:v>
+                </c:pt>
+                <c:pt idx="971">
+                  <c:v>97200</c:v>
+                </c:pt>
+                <c:pt idx="972">
+                  <c:v>97300</c:v>
+                </c:pt>
+                <c:pt idx="973">
+                  <c:v>97400</c:v>
+                </c:pt>
+                <c:pt idx="974">
+                  <c:v>97500</c:v>
+                </c:pt>
+                <c:pt idx="975">
+                  <c:v>97600</c:v>
+                </c:pt>
+                <c:pt idx="976">
+                  <c:v>97700</c:v>
+                </c:pt>
+                <c:pt idx="977">
+                  <c:v>97800</c:v>
+                </c:pt>
+                <c:pt idx="978">
+                  <c:v>97900</c:v>
+                </c:pt>
+                <c:pt idx="979">
+                  <c:v>98000</c:v>
+                </c:pt>
+                <c:pt idx="980">
+                  <c:v>98100</c:v>
+                </c:pt>
+                <c:pt idx="981">
+                  <c:v>98200</c:v>
+                </c:pt>
+                <c:pt idx="982">
+                  <c:v>98300</c:v>
+                </c:pt>
+                <c:pt idx="983">
+                  <c:v>98400</c:v>
+                </c:pt>
+                <c:pt idx="984">
+                  <c:v>98500</c:v>
+                </c:pt>
+                <c:pt idx="985">
+                  <c:v>98600</c:v>
+                </c:pt>
+                <c:pt idx="986">
+                  <c:v>98700</c:v>
+                </c:pt>
+                <c:pt idx="987">
+                  <c:v>98800</c:v>
+                </c:pt>
+                <c:pt idx="988">
+                  <c:v>98900</c:v>
+                </c:pt>
+                <c:pt idx="989">
+                  <c:v>99000</c:v>
+                </c:pt>
+                <c:pt idx="990">
+                  <c:v>99100</c:v>
+                </c:pt>
+                <c:pt idx="991">
+                  <c:v>99200</c:v>
+                </c:pt>
+                <c:pt idx="992">
+                  <c:v>99300</c:v>
+                </c:pt>
+                <c:pt idx="993">
+                  <c:v>99400</c:v>
+                </c:pt>
+                <c:pt idx="994">
+                  <c:v>99500</c:v>
+                </c:pt>
+                <c:pt idx="995">
+                  <c:v>99600</c:v>
+                </c:pt>
+                <c:pt idx="996">
+                  <c:v>99700</c:v>
+                </c:pt>
+                <c:pt idx="997">
+                  <c:v>99800</c:v>
+                </c:pt>
+                <c:pt idx="998">
+                  <c:v>99900</c:v>
+                </c:pt>
+                <c:pt idx="999">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$839</c:f>
+              <c:f>Sheet1!$C$2:$C$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="838"/>
+                <c:ptCount val="1000"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-16BF-4A92-9F12-241668F6DF81}"/>
+              <c16:uniqueId val="{00000001-4C15-459C-B3ED-C7353D9B3358}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7808,10 +9286,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$839</c:f>
+              <c:f>Sheet1!$A$2:$A$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="838"/>
+                <c:ptCount val="1000"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -10325,16 +11803,502 @@
                 </c:pt>
                 <c:pt idx="837">
                   <c:v>83800</c:v>
+                </c:pt>
+                <c:pt idx="838">
+                  <c:v>83900</c:v>
+                </c:pt>
+                <c:pt idx="839">
+                  <c:v>84000</c:v>
+                </c:pt>
+                <c:pt idx="840">
+                  <c:v>84100</c:v>
+                </c:pt>
+                <c:pt idx="841">
+                  <c:v>84200</c:v>
+                </c:pt>
+                <c:pt idx="842">
+                  <c:v>84300</c:v>
+                </c:pt>
+                <c:pt idx="843">
+                  <c:v>84400</c:v>
+                </c:pt>
+                <c:pt idx="844">
+                  <c:v>84500</c:v>
+                </c:pt>
+                <c:pt idx="845">
+                  <c:v>84600</c:v>
+                </c:pt>
+                <c:pt idx="846">
+                  <c:v>84700</c:v>
+                </c:pt>
+                <c:pt idx="847">
+                  <c:v>84800</c:v>
+                </c:pt>
+                <c:pt idx="848">
+                  <c:v>84900</c:v>
+                </c:pt>
+                <c:pt idx="849">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="850">
+                  <c:v>85100</c:v>
+                </c:pt>
+                <c:pt idx="851">
+                  <c:v>85200</c:v>
+                </c:pt>
+                <c:pt idx="852">
+                  <c:v>85300</c:v>
+                </c:pt>
+                <c:pt idx="853">
+                  <c:v>85400</c:v>
+                </c:pt>
+                <c:pt idx="854">
+                  <c:v>85500</c:v>
+                </c:pt>
+                <c:pt idx="855">
+                  <c:v>85600</c:v>
+                </c:pt>
+                <c:pt idx="856">
+                  <c:v>85700</c:v>
+                </c:pt>
+                <c:pt idx="857">
+                  <c:v>85800</c:v>
+                </c:pt>
+                <c:pt idx="858">
+                  <c:v>85900</c:v>
+                </c:pt>
+                <c:pt idx="859">
+                  <c:v>86000</c:v>
+                </c:pt>
+                <c:pt idx="860">
+                  <c:v>86100</c:v>
+                </c:pt>
+                <c:pt idx="861">
+                  <c:v>86200</c:v>
+                </c:pt>
+                <c:pt idx="862">
+                  <c:v>86300</c:v>
+                </c:pt>
+                <c:pt idx="863">
+                  <c:v>86400</c:v>
+                </c:pt>
+                <c:pt idx="864">
+                  <c:v>86500</c:v>
+                </c:pt>
+                <c:pt idx="865">
+                  <c:v>86600</c:v>
+                </c:pt>
+                <c:pt idx="866">
+                  <c:v>86700</c:v>
+                </c:pt>
+                <c:pt idx="867">
+                  <c:v>86800</c:v>
+                </c:pt>
+                <c:pt idx="868">
+                  <c:v>86900</c:v>
+                </c:pt>
+                <c:pt idx="869">
+                  <c:v>87000</c:v>
+                </c:pt>
+                <c:pt idx="870">
+                  <c:v>87100</c:v>
+                </c:pt>
+                <c:pt idx="871">
+                  <c:v>87200</c:v>
+                </c:pt>
+                <c:pt idx="872">
+                  <c:v>87300</c:v>
+                </c:pt>
+                <c:pt idx="873">
+                  <c:v>87400</c:v>
+                </c:pt>
+                <c:pt idx="874">
+                  <c:v>87500</c:v>
+                </c:pt>
+                <c:pt idx="875">
+                  <c:v>87600</c:v>
+                </c:pt>
+                <c:pt idx="876">
+                  <c:v>87700</c:v>
+                </c:pt>
+                <c:pt idx="877">
+                  <c:v>87800</c:v>
+                </c:pt>
+                <c:pt idx="878">
+                  <c:v>87900</c:v>
+                </c:pt>
+                <c:pt idx="879">
+                  <c:v>88000</c:v>
+                </c:pt>
+                <c:pt idx="880">
+                  <c:v>88100</c:v>
+                </c:pt>
+                <c:pt idx="881">
+                  <c:v>88200</c:v>
+                </c:pt>
+                <c:pt idx="882">
+                  <c:v>88300</c:v>
+                </c:pt>
+                <c:pt idx="883">
+                  <c:v>88400</c:v>
+                </c:pt>
+                <c:pt idx="884">
+                  <c:v>88500</c:v>
+                </c:pt>
+                <c:pt idx="885">
+                  <c:v>88600</c:v>
+                </c:pt>
+                <c:pt idx="886">
+                  <c:v>88700</c:v>
+                </c:pt>
+                <c:pt idx="887">
+                  <c:v>88800</c:v>
+                </c:pt>
+                <c:pt idx="888">
+                  <c:v>88900</c:v>
+                </c:pt>
+                <c:pt idx="889">
+                  <c:v>89000</c:v>
+                </c:pt>
+                <c:pt idx="890">
+                  <c:v>89100</c:v>
+                </c:pt>
+                <c:pt idx="891">
+                  <c:v>89200</c:v>
+                </c:pt>
+                <c:pt idx="892">
+                  <c:v>89300</c:v>
+                </c:pt>
+                <c:pt idx="893">
+                  <c:v>89400</c:v>
+                </c:pt>
+                <c:pt idx="894">
+                  <c:v>89500</c:v>
+                </c:pt>
+                <c:pt idx="895">
+                  <c:v>89600</c:v>
+                </c:pt>
+                <c:pt idx="896">
+                  <c:v>89700</c:v>
+                </c:pt>
+                <c:pt idx="897">
+                  <c:v>89800</c:v>
+                </c:pt>
+                <c:pt idx="898">
+                  <c:v>89900</c:v>
+                </c:pt>
+                <c:pt idx="899">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="900">
+                  <c:v>90100</c:v>
+                </c:pt>
+                <c:pt idx="901">
+                  <c:v>90200</c:v>
+                </c:pt>
+                <c:pt idx="902">
+                  <c:v>90300</c:v>
+                </c:pt>
+                <c:pt idx="903">
+                  <c:v>90400</c:v>
+                </c:pt>
+                <c:pt idx="904">
+                  <c:v>90500</c:v>
+                </c:pt>
+                <c:pt idx="905">
+                  <c:v>90600</c:v>
+                </c:pt>
+                <c:pt idx="906">
+                  <c:v>90700</c:v>
+                </c:pt>
+                <c:pt idx="907">
+                  <c:v>90800</c:v>
+                </c:pt>
+                <c:pt idx="908">
+                  <c:v>90900</c:v>
+                </c:pt>
+                <c:pt idx="909">
+                  <c:v>91000</c:v>
+                </c:pt>
+                <c:pt idx="910">
+                  <c:v>91100</c:v>
+                </c:pt>
+                <c:pt idx="911">
+                  <c:v>91200</c:v>
+                </c:pt>
+                <c:pt idx="912">
+                  <c:v>91300</c:v>
+                </c:pt>
+                <c:pt idx="913">
+                  <c:v>91400</c:v>
+                </c:pt>
+                <c:pt idx="914">
+                  <c:v>91500</c:v>
+                </c:pt>
+                <c:pt idx="915">
+                  <c:v>91600</c:v>
+                </c:pt>
+                <c:pt idx="916">
+                  <c:v>91700</c:v>
+                </c:pt>
+                <c:pt idx="917">
+                  <c:v>91800</c:v>
+                </c:pt>
+                <c:pt idx="918">
+                  <c:v>91900</c:v>
+                </c:pt>
+                <c:pt idx="919">
+                  <c:v>92000</c:v>
+                </c:pt>
+                <c:pt idx="920">
+                  <c:v>92100</c:v>
+                </c:pt>
+                <c:pt idx="921">
+                  <c:v>92200</c:v>
+                </c:pt>
+                <c:pt idx="922">
+                  <c:v>92300</c:v>
+                </c:pt>
+                <c:pt idx="923">
+                  <c:v>92400</c:v>
+                </c:pt>
+                <c:pt idx="924">
+                  <c:v>92500</c:v>
+                </c:pt>
+                <c:pt idx="925">
+                  <c:v>92600</c:v>
+                </c:pt>
+                <c:pt idx="926">
+                  <c:v>92700</c:v>
+                </c:pt>
+                <c:pt idx="927">
+                  <c:v>92800</c:v>
+                </c:pt>
+                <c:pt idx="928">
+                  <c:v>92900</c:v>
+                </c:pt>
+                <c:pt idx="929">
+                  <c:v>93000</c:v>
+                </c:pt>
+                <c:pt idx="930">
+                  <c:v>93100</c:v>
+                </c:pt>
+                <c:pt idx="931">
+                  <c:v>93200</c:v>
+                </c:pt>
+                <c:pt idx="932">
+                  <c:v>93300</c:v>
+                </c:pt>
+                <c:pt idx="933">
+                  <c:v>93400</c:v>
+                </c:pt>
+                <c:pt idx="934">
+                  <c:v>93500</c:v>
+                </c:pt>
+                <c:pt idx="935">
+                  <c:v>93600</c:v>
+                </c:pt>
+                <c:pt idx="936">
+                  <c:v>93700</c:v>
+                </c:pt>
+                <c:pt idx="937">
+                  <c:v>93800</c:v>
+                </c:pt>
+                <c:pt idx="938">
+                  <c:v>93900</c:v>
+                </c:pt>
+                <c:pt idx="939">
+                  <c:v>94000</c:v>
+                </c:pt>
+                <c:pt idx="940">
+                  <c:v>94100</c:v>
+                </c:pt>
+                <c:pt idx="941">
+                  <c:v>94200</c:v>
+                </c:pt>
+                <c:pt idx="942">
+                  <c:v>94300</c:v>
+                </c:pt>
+                <c:pt idx="943">
+                  <c:v>94400</c:v>
+                </c:pt>
+                <c:pt idx="944">
+                  <c:v>94500</c:v>
+                </c:pt>
+                <c:pt idx="945">
+                  <c:v>94600</c:v>
+                </c:pt>
+                <c:pt idx="946">
+                  <c:v>94700</c:v>
+                </c:pt>
+                <c:pt idx="947">
+                  <c:v>94800</c:v>
+                </c:pt>
+                <c:pt idx="948">
+                  <c:v>94900</c:v>
+                </c:pt>
+                <c:pt idx="949">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="950">
+                  <c:v>95100</c:v>
+                </c:pt>
+                <c:pt idx="951">
+                  <c:v>95200</c:v>
+                </c:pt>
+                <c:pt idx="952">
+                  <c:v>95300</c:v>
+                </c:pt>
+                <c:pt idx="953">
+                  <c:v>95400</c:v>
+                </c:pt>
+                <c:pt idx="954">
+                  <c:v>95500</c:v>
+                </c:pt>
+                <c:pt idx="955">
+                  <c:v>95600</c:v>
+                </c:pt>
+                <c:pt idx="956">
+                  <c:v>95700</c:v>
+                </c:pt>
+                <c:pt idx="957">
+                  <c:v>95800</c:v>
+                </c:pt>
+                <c:pt idx="958">
+                  <c:v>95900</c:v>
+                </c:pt>
+                <c:pt idx="959">
+                  <c:v>96000</c:v>
+                </c:pt>
+                <c:pt idx="960">
+                  <c:v>96100</c:v>
+                </c:pt>
+                <c:pt idx="961">
+                  <c:v>96200</c:v>
+                </c:pt>
+                <c:pt idx="962">
+                  <c:v>96300</c:v>
+                </c:pt>
+                <c:pt idx="963">
+                  <c:v>96400</c:v>
+                </c:pt>
+                <c:pt idx="964">
+                  <c:v>96500</c:v>
+                </c:pt>
+                <c:pt idx="965">
+                  <c:v>96600</c:v>
+                </c:pt>
+                <c:pt idx="966">
+                  <c:v>96700</c:v>
+                </c:pt>
+                <c:pt idx="967">
+                  <c:v>96800</c:v>
+                </c:pt>
+                <c:pt idx="968">
+                  <c:v>96900</c:v>
+                </c:pt>
+                <c:pt idx="969">
+                  <c:v>97000</c:v>
+                </c:pt>
+                <c:pt idx="970">
+                  <c:v>97100</c:v>
+                </c:pt>
+                <c:pt idx="971">
+                  <c:v>97200</c:v>
+                </c:pt>
+                <c:pt idx="972">
+                  <c:v>97300</c:v>
+                </c:pt>
+                <c:pt idx="973">
+                  <c:v>97400</c:v>
+                </c:pt>
+                <c:pt idx="974">
+                  <c:v>97500</c:v>
+                </c:pt>
+                <c:pt idx="975">
+                  <c:v>97600</c:v>
+                </c:pt>
+                <c:pt idx="976">
+                  <c:v>97700</c:v>
+                </c:pt>
+                <c:pt idx="977">
+                  <c:v>97800</c:v>
+                </c:pt>
+                <c:pt idx="978">
+                  <c:v>97900</c:v>
+                </c:pt>
+                <c:pt idx="979">
+                  <c:v>98000</c:v>
+                </c:pt>
+                <c:pt idx="980">
+                  <c:v>98100</c:v>
+                </c:pt>
+                <c:pt idx="981">
+                  <c:v>98200</c:v>
+                </c:pt>
+                <c:pt idx="982">
+                  <c:v>98300</c:v>
+                </c:pt>
+                <c:pt idx="983">
+                  <c:v>98400</c:v>
+                </c:pt>
+                <c:pt idx="984">
+                  <c:v>98500</c:v>
+                </c:pt>
+                <c:pt idx="985">
+                  <c:v>98600</c:v>
+                </c:pt>
+                <c:pt idx="986">
+                  <c:v>98700</c:v>
+                </c:pt>
+                <c:pt idx="987">
+                  <c:v>98800</c:v>
+                </c:pt>
+                <c:pt idx="988">
+                  <c:v>98900</c:v>
+                </c:pt>
+                <c:pt idx="989">
+                  <c:v>99000</c:v>
+                </c:pt>
+                <c:pt idx="990">
+                  <c:v>99100</c:v>
+                </c:pt>
+                <c:pt idx="991">
+                  <c:v>99200</c:v>
+                </c:pt>
+                <c:pt idx="992">
+                  <c:v>99300</c:v>
+                </c:pt>
+                <c:pt idx="993">
+                  <c:v>99400</c:v>
+                </c:pt>
+                <c:pt idx="994">
+                  <c:v>99500</c:v>
+                </c:pt>
+                <c:pt idx="995">
+                  <c:v>99600</c:v>
+                </c:pt>
+                <c:pt idx="996">
+                  <c:v>99700</c:v>
+                </c:pt>
+                <c:pt idx="997">
+                  <c:v>99800</c:v>
+                </c:pt>
+                <c:pt idx="998">
+                  <c:v>99900</c:v>
+                </c:pt>
+                <c:pt idx="999">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$839</c:f>
+              <c:f>Sheet1!$D$2:$D$1001</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="838"/>
+                <c:ptCount val="1000"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -12848,14 +14812,500 @@
                 </c:pt>
                 <c:pt idx="837">
                   <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="838">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="839">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="840">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="841">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="842">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="843">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="844">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="845">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="846">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="847">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="848">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="849">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="850">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="851">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="852">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="853">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="854">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="855">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="856">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="857">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="858">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="859">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="860">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="861">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="862">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="863">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="864">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="865">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="866">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="867">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="868">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="869">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="870">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="871">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="872">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="873">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="874">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="875">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="876">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="877">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="878">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="879">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="880">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="881">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="882">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="883">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="884">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="885">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="886">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="887">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="888">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="889">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="890">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="891">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="892">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="893">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="894">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="895">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="896">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="897">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="898">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="899">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="900">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="901">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="902">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="903">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="904">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="905">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="906">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="907">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="908">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="909">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="910">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="911">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="912">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="913">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="914">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="915">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="916">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="917">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="918">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="919">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="920">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="921">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="922">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="923">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="924">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="925">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="926">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="927">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="928">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="929">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="930">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="931">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="932">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="933">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="934">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="935">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="936">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="937">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="938">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="939">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="940">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="941">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="942">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="943">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="944">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="945">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="946">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="947">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="948">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="949">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="950">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="951">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="952">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="953">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="954">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="955">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="956">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="957">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="958">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="959">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="960">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="961">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="962">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="963">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="964">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="965">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="966">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="967">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="968">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="969">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="970">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="971">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="972">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="973">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="974">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="975">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="976">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="977">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="978">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="979">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="980">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="981">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="982">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="983">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="984">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="985">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="986">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="987">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="988">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="989">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="990">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="991">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="992">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="993">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="994">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="995">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="996">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="997">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="998">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="999">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-16BF-4A92-9F12-241668F6DF81}"/>
+              <c16:uniqueId val="{00000002-4C15-459C-B3ED-C7353D9B3358}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -12867,11 +15317,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="275424848"/>
-        <c:axId val="275433168"/>
+        <c:axId val="457511711"/>
+        <c:axId val="457516511"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="275424848"/>
+        <c:axId val="457511711"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12928,12 +15378,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275433168"/>
+        <c:crossAx val="457516511"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="275433168"/>
+        <c:axId val="457516511"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12990,7 +15440,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="275424848"/>
+        <c:crossAx val="457511711"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13004,10 +15454,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:legendEntry>
-        <c:idx val="1"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13641,23 +16087,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>358557</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>122903</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>402363</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>102549</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>114908</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>122903</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>505625</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>28486</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Chart 12">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9290B69-4269-FF84-4FFC-6AAA30935D51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8C62DCF-1E3C-EE02-66E4-D8E0662170CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13977,8 +16423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA6E512-6B6E-4574-8D35-36D08849DBD1}">
   <dimension ref="A1:E1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="X32" sqref="X32"/>
+    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>